<commit_message>
Sd add MS dans les profils ROR (#269)
* add MS d8e684dbb73dc13f9db8dd97eaab29e3d6920d3b
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-ror-healthcareservice.xlsx
+++ b/main/ig/StructureDefinition-ror-healthcareservice.xlsx
@@ -9,6 +9,9 @@
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AL$177</definedName>
+  </definedNames>
 </workbook>
 </file>
 
@@ -54,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-07T11:08:45+00:00</t>
+    <t>2024-02-07T14:28:15+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -2231,6 +2234,21 @@
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="22"/>
+        <i val="true"/>
+      </font>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -2569,7 +2587,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" hidden="true">
       <c r="A2" t="s" s="2">
         <v>29</v>
       </c>
@@ -2675,7 +2693,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
         <v>82</v>
       </c>
@@ -2783,7 +2801,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" hidden="true">
       <c r="A4" t="s" s="2">
         <v>90</v>
       </c>
@@ -2889,7 +2907,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
         <v>98</v>
       </c>
@@ -2995,7 +3013,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
         <v>104</v>
       </c>
@@ -3103,7 +3121,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
         <v>115</v>
       </c>
@@ -3211,7 +3229,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
         <v>120</v>
       </c>
@@ -3230,7 +3248,7 @@
         <v>83</v>
       </c>
       <c r="H8" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I8" t="s" s="2">
         <v>74</v>
@@ -3319,7 +3337,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
         <v>126</v>
       </c>
@@ -3427,7 +3445,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
         <v>132</v>
       </c>
@@ -3535,7 +3553,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
         <v>138</v>
       </c>
@@ -3643,7 +3661,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
         <v>148</v>
       </c>
@@ -3751,7 +3769,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
         <v>157</v>
       </c>
@@ -3772,7 +3790,7 @@
         <v>83</v>
       </c>
       <c r="H13" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I13" t="s" s="2">
         <v>74</v>
@@ -3859,7 +3877,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
         <v>161</v>
       </c>
@@ -3967,7 +3985,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
         <v>166</v>
       </c>
@@ -4075,7 +4093,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
         <v>175</v>
       </c>
@@ -4183,7 +4201,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
         <v>183</v>
       </c>
@@ -4291,7 +4309,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
         <v>190</v>
       </c>
@@ -4397,7 +4415,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
         <v>195</v>
       </c>
@@ -4418,7 +4436,7 @@
         <v>76</v>
       </c>
       <c r="H19" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I19" t="s" s="2">
         <v>74</v>
@@ -4505,7 +4523,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
         <v>200</v>
       </c>
@@ -4526,7 +4544,7 @@
         <v>83</v>
       </c>
       <c r="H20" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I20" t="s" s="2">
         <v>74</v>
@@ -4613,7 +4631,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
         <v>205</v>
       </c>
@@ -4634,7 +4652,7 @@
         <v>83</v>
       </c>
       <c r="H21" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I21" t="s" s="2">
         <v>74</v>
@@ -4721,7 +4739,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
         <v>210</v>
       </c>
@@ -4742,7 +4760,7 @@
         <v>76</v>
       </c>
       <c r="H22" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I22" t="s" s="2">
         <v>74</v>
@@ -4829,7 +4847,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
         <v>215</v>
       </c>
@@ -4850,7 +4868,7 @@
         <v>83</v>
       </c>
       <c r="H23" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I23" t="s" s="2">
         <v>74</v>
@@ -4937,7 +4955,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
         <v>220</v>
       </c>
@@ -4958,7 +4976,7 @@
         <v>76</v>
       </c>
       <c r="H24" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I24" t="s" s="2">
         <v>74</v>
@@ -5045,7 +5063,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
         <v>225</v>
       </c>
@@ -5066,7 +5084,7 @@
         <v>83</v>
       </c>
       <c r="H25" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I25" t="s" s="2">
         <v>74</v>
@@ -5153,7 +5171,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
         <v>230</v>
       </c>
@@ -5263,7 +5281,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
         <v>235</v>
       </c>
@@ -5282,7 +5300,7 @@
         <v>83</v>
       </c>
       <c r="H27" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I27" t="s" s="2">
         <v>74</v>
@@ -5369,7 +5387,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
         <v>241</v>
       </c>
@@ -5479,7 +5497,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
         <v>249</v>
       </c>
@@ -5498,7 +5516,7 @@
         <v>83</v>
       </c>
       <c r="H29" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I29" t="s" s="2">
         <v>74</v>
@@ -5587,7 +5605,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
         <v>256</v>
       </c>
@@ -5606,7 +5624,7 @@
         <v>83</v>
       </c>
       <c r="H30" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I30" t="s" s="2">
         <v>74</v>
@@ -5693,7 +5711,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
         <v>265</v>
       </c>
@@ -5712,7 +5730,7 @@
         <v>83</v>
       </c>
       <c r="H31" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I31" t="s" s="2">
         <v>74</v>
@@ -5799,7 +5817,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
         <v>272</v>
       </c>
@@ -5818,7 +5836,7 @@
         <v>76</v>
       </c>
       <c r="H32" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I32" t="s" s="2">
         <v>74</v>
@@ -5905,7 +5923,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
         <v>278</v>
       </c>
@@ -5926,7 +5944,7 @@
         <v>83</v>
       </c>
       <c r="H33" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I33" t="s" s="2">
         <v>74</v>
@@ -6013,7 +6031,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
         <v>282</v>
       </c>
@@ -6034,7 +6052,7 @@
         <v>83</v>
       </c>
       <c r="H34" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I34" t="s" s="2">
         <v>74</v>
@@ -6121,7 +6139,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
         <v>286</v>
       </c>
@@ -6140,7 +6158,7 @@
         <v>76</v>
       </c>
       <c r="H35" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I35" t="s" s="2">
         <v>74</v>
@@ -6229,7 +6247,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
         <v>293</v>
       </c>
@@ -6248,7 +6266,7 @@
         <v>83</v>
       </c>
       <c r="H36" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I36" t="s" s="2">
         <v>74</v>
@@ -6337,7 +6355,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
         <v>298</v>
       </c>
@@ -6445,7 +6463,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
         <v>303</v>
       </c>
@@ -6553,7 +6571,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
         <v>309</v>
       </c>
@@ -6661,7 +6679,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
         <v>316</v>
       </c>
@@ -6769,7 +6787,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
         <v>323</v>
       </c>
@@ -6875,7 +6893,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
         <v>324</v>
       </c>
@@ -6981,7 +6999,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
         <v>326</v>
       </c>
@@ -7002,7 +7020,7 @@
         <v>83</v>
       </c>
       <c r="H43" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I43" t="s" s="2">
         <v>74</v>
@@ -7089,7 +7107,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
         <v>331</v>
       </c>
@@ -7110,7 +7128,7 @@
         <v>83</v>
       </c>
       <c r="H44" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I44" t="s" s="2">
         <v>74</v>
@@ -7197,7 +7215,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
         <v>336</v>
       </c>
@@ -7218,7 +7236,7 @@
         <v>83</v>
       </c>
       <c r="H45" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I45" t="s" s="2">
         <v>74</v>
@@ -7305,7 +7323,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
         <v>341</v>
       </c>
@@ -7413,7 +7431,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
         <v>349</v>
       </c>
@@ -7432,7 +7450,7 @@
         <v>83</v>
       </c>
       <c r="H47" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I47" t="s" s="2">
         <v>74</v>
@@ -7523,7 +7541,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
         <v>356</v>
       </c>
@@ -7633,7 +7651,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
         <v>365</v>
       </c>
@@ -7741,7 +7759,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
         <v>371</v>
       </c>
@@ -7849,7 +7867,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
         <v>379</v>
       </c>
@@ -7957,7 +7975,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
         <v>384</v>
       </c>
@@ -8065,7 +8083,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
         <v>390</v>
       </c>
@@ -8171,7 +8189,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
         <v>394</v>
       </c>
@@ -8277,7 +8295,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
         <v>395</v>
       </c>
@@ -8385,7 +8403,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
         <v>396</v>
       </c>
@@ -8495,7 +8513,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
         <v>401</v>
       </c>
@@ -8603,7 +8621,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
         <v>405</v>
       </c>
@@ -8711,7 +8729,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
         <v>410</v>
       </c>
@@ -8819,7 +8837,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
         <v>417</v>
       </c>
@@ -8838,7 +8856,7 @@
         <v>76</v>
       </c>
       <c r="H60" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I60" t="s" s="2">
         <v>74</v>
@@ -8925,7 +8943,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
         <v>423</v>
       </c>
@@ -9031,7 +9049,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
         <v>424</v>
       </c>
@@ -9139,7 +9157,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
         <v>425</v>
       </c>
@@ -9160,7 +9178,7 @@
         <v>83</v>
       </c>
       <c r="H63" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I63" t="s" s="2">
         <v>74</v>
@@ -9247,7 +9265,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
         <v>430</v>
       </c>
@@ -9357,7 +9375,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
         <v>437</v>
       </c>
@@ -9467,7 +9485,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
         <v>444</v>
       </c>
@@ -9488,7 +9506,7 @@
         <v>83</v>
       </c>
       <c r="H66" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I66" t="s" s="2">
         <v>74</v>
@@ -9575,7 +9593,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
         <v>448</v>
       </c>
@@ -9681,7 +9699,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
         <v>449</v>
       </c>
@@ -9789,7 +9807,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
         <v>450</v>
       </c>
@@ -9810,7 +9828,7 @@
         <v>75</v>
       </c>
       <c r="H69" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I69" t="s" s="2">
         <v>74</v>
@@ -9897,7 +9915,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
         <v>451</v>
       </c>
@@ -10007,7 +10025,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
         <v>452</v>
       </c>
@@ -10117,7 +10135,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
         <v>453</v>
       </c>
@@ -10138,7 +10156,7 @@
         <v>83</v>
       </c>
       <c r="H72" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I72" t="s" s="2">
         <v>74</v>
@@ -10225,7 +10243,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
         <v>457</v>
       </c>
@@ -10331,7 +10349,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
         <v>458</v>
       </c>
@@ -10439,7 +10457,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
         <v>459</v>
       </c>
@@ -10460,7 +10478,7 @@
         <v>75</v>
       </c>
       <c r="H75" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I75" t="s" s="2">
         <v>74</v>
@@ -10547,7 +10565,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
         <v>460</v>
       </c>
@@ -10657,7 +10675,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
         <v>461</v>
       </c>
@@ -10767,7 +10785,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
         <v>462</v>
       </c>
@@ -10788,7 +10806,7 @@
         <v>76</v>
       </c>
       <c r="H78" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I78" t="s" s="2">
         <v>74</v>
@@ -10875,7 +10893,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
         <v>466</v>
       </c>
@@ -10981,7 +10999,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
         <v>467</v>
       </c>
@@ -11089,7 +11107,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
         <v>468</v>
       </c>
@@ -11110,7 +11128,7 @@
         <v>75</v>
       </c>
       <c r="H81" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I81" t="s" s="2">
         <v>74</v>
@@ -11197,7 +11215,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="82">
+    <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
         <v>469</v>
       </c>
@@ -11307,7 +11325,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
         <v>470</v>
       </c>
@@ -11417,7 +11435,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
         <v>471</v>
       </c>
@@ -11438,7 +11456,7 @@
         <v>76</v>
       </c>
       <c r="H84" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I84" t="s" s="2">
         <v>74</v>
@@ -11525,7 +11543,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
         <v>475</v>
       </c>
@@ -11631,7 +11649,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
         <v>476</v>
       </c>
@@ -11739,7 +11757,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
         <v>477</v>
       </c>
@@ -11760,7 +11778,7 @@
         <v>75</v>
       </c>
       <c r="H87" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I87" t="s" s="2">
         <v>74</v>
@@ -11847,7 +11865,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="88">
+    <row r="88" hidden="true">
       <c r="A88" t="s" s="2">
         <v>478</v>
       </c>
@@ -11957,7 +11975,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="89">
+    <row r="89" hidden="true">
       <c r="A89" t="s" s="2">
         <v>479</v>
       </c>
@@ -12067,7 +12085,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="90">
+    <row r="90" hidden="true">
       <c r="A90" t="s" s="2">
         <v>480</v>
       </c>
@@ -12088,7 +12106,7 @@
         <v>76</v>
       </c>
       <c r="H90" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I90" t="s" s="2">
         <v>74</v>
@@ -12175,7 +12193,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" hidden="true">
       <c r="A91" t="s" s="2">
         <v>484</v>
       </c>
@@ -12281,7 +12299,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" hidden="true">
       <c r="A92" t="s" s="2">
         <v>485</v>
       </c>
@@ -12387,7 +12405,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="93">
+    <row r="93" hidden="true">
       <c r="A93" t="s" s="2">
         <v>486</v>
       </c>
@@ -12408,7 +12426,7 @@
         <v>83</v>
       </c>
       <c r="H93" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I93" t="s" s="2">
         <v>74</v>
@@ -12495,7 +12513,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="94">
+    <row r="94" hidden="true">
       <c r="A94" t="s" s="2">
         <v>487</v>
       </c>
@@ -12601,7 +12619,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="95">
+    <row r="95" hidden="true">
       <c r="A95" t="s" s="2">
         <v>489</v>
       </c>
@@ -12707,7 +12725,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="96">
+    <row r="96" hidden="true">
       <c r="A96" t="s" s="2">
         <v>491</v>
       </c>
@@ -12815,7 +12833,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="97">
+    <row r="97" hidden="true">
       <c r="A97" t="s" s="2">
         <v>498</v>
       </c>
@@ -12919,7 +12937,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" hidden="true">
       <c r="A98" t="s" s="2">
         <v>504</v>
       </c>
@@ -13029,7 +13047,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" hidden="true">
       <c r="A99" t="s" s="2">
         <v>505</v>
       </c>
@@ -13139,7 +13157,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="100">
+    <row r="100" hidden="true">
       <c r="A100" t="s" s="2">
         <v>506</v>
       </c>
@@ -13160,7 +13178,7 @@
         <v>76</v>
       </c>
       <c r="H100" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I100" t="s" s="2">
         <v>74</v>
@@ -13247,7 +13265,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" hidden="true">
       <c r="A101" t="s" s="2">
         <v>509</v>
       </c>
@@ -13353,7 +13371,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" hidden="true">
       <c r="A102" t="s" s="2">
         <v>510</v>
       </c>
@@ -13459,7 +13477,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" hidden="true">
       <c r="A103" t="s" s="2">
         <v>511</v>
       </c>
@@ -13480,7 +13498,7 @@
         <v>83</v>
       </c>
       <c r="H103" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I103" t="s" s="2">
         <v>74</v>
@@ -13567,7 +13585,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" hidden="true">
       <c r="A104" t="s" s="2">
         <v>512</v>
       </c>
@@ -13673,7 +13691,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" hidden="true">
       <c r="A105" t="s" s="2">
         <v>513</v>
       </c>
@@ -13779,7 +13797,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" hidden="true">
       <c r="A106" t="s" s="2">
         <v>514</v>
       </c>
@@ -13887,7 +13905,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" hidden="true">
       <c r="A107" t="s" s="2">
         <v>515</v>
       </c>
@@ -13991,7 +14009,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" hidden="true">
       <c r="A108" t="s" s="2">
         <v>516</v>
       </c>
@@ -14101,7 +14119,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" hidden="true">
       <c r="A109" t="s" s="2">
         <v>517</v>
       </c>
@@ -14211,7 +14229,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" hidden="true">
       <c r="A110" t="s" s="2">
         <v>518</v>
       </c>
@@ -14232,7 +14250,7 @@
         <v>76</v>
       </c>
       <c r="H110" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I110" t="s" s="2">
         <v>74</v>
@@ -14319,7 +14337,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" hidden="true">
       <c r="A111" t="s" s="2">
         <v>522</v>
       </c>
@@ -14425,7 +14443,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" hidden="true">
       <c r="A112" t="s" s="2">
         <v>523</v>
       </c>
@@ -14533,7 +14551,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" hidden="true">
       <c r="A113" t="s" s="2">
         <v>524</v>
       </c>
@@ -14554,7 +14572,7 @@
         <v>75</v>
       </c>
       <c r="H113" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I113" t="s" s="2">
         <v>74</v>
@@ -14641,7 +14659,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" hidden="true">
       <c r="A114" t="s" s="2">
         <v>525</v>
       </c>
@@ -14751,7 +14769,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" hidden="true">
       <c r="A115" t="s" s="2">
         <v>526</v>
       </c>
@@ -14861,7 +14879,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" hidden="true">
       <c r="A116" t="s" s="2">
         <v>527</v>
       </c>
@@ -14882,7 +14900,7 @@
         <v>83</v>
       </c>
       <c r="H116" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I116" t="s" s="2">
         <v>74</v>
@@ -14969,7 +14987,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" hidden="true">
       <c r="A117" t="s" s="2">
         <v>531</v>
       </c>
@@ -15075,7 +15093,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" hidden="true">
       <c r="A118" t="s" s="2">
         <v>532</v>
       </c>
@@ -15183,7 +15201,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" hidden="true">
       <c r="A119" t="s" s="2">
         <v>533</v>
       </c>
@@ -15204,7 +15222,7 @@
         <v>75</v>
       </c>
       <c r="H119" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I119" t="s" s="2">
         <v>74</v>
@@ -15291,7 +15309,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" hidden="true">
       <c r="A120" t="s" s="2">
         <v>534</v>
       </c>
@@ -15401,7 +15419,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="121">
+    <row r="121" hidden="true">
       <c r="A121" t="s" s="2">
         <v>535</v>
       </c>
@@ -15511,7 +15529,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="122">
+    <row r="122" hidden="true">
       <c r="A122" t="s" s="2">
         <v>536</v>
       </c>
@@ -15532,7 +15550,7 @@
         <v>76</v>
       </c>
       <c r="H122" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I122" t="s" s="2">
         <v>74</v>
@@ -15619,7 +15637,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" hidden="true">
       <c r="A123" t="s" s="2">
         <v>540</v>
       </c>
@@ -15725,7 +15743,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="124">
+    <row r="124" hidden="true">
       <c r="A124" t="s" s="2">
         <v>541</v>
       </c>
@@ -15833,7 +15851,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="125">
+    <row r="125" hidden="true">
       <c r="A125" t="s" s="2">
         <v>542</v>
       </c>
@@ -15854,7 +15872,7 @@
         <v>75</v>
       </c>
       <c r="H125" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I125" t="s" s="2">
         <v>74</v>
@@ -15941,7 +15959,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="126">
+    <row r="126" hidden="true">
       <c r="A126" t="s" s="2">
         <v>543</v>
       </c>
@@ -16051,7 +16069,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="127">
+    <row r="127" hidden="true">
       <c r="A127" t="s" s="2">
         <v>544</v>
       </c>
@@ -16161,7 +16179,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="128">
+    <row r="128" hidden="true">
       <c r="A128" t="s" s="2">
         <v>545</v>
       </c>
@@ -16182,7 +16200,7 @@
         <v>76</v>
       </c>
       <c r="H128" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I128" t="s" s="2">
         <v>74</v>
@@ -16269,7 +16287,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="129">
+    <row r="129" hidden="true">
       <c r="A129" t="s" s="2">
         <v>549</v>
       </c>
@@ -16375,7 +16393,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="130">
+    <row r="130" hidden="true">
       <c r="A130" t="s" s="2">
         <v>550</v>
       </c>
@@ -16483,7 +16501,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="131">
+    <row r="131" hidden="true">
       <c r="A131" t="s" s="2">
         <v>551</v>
       </c>
@@ -16504,7 +16522,7 @@
         <v>75</v>
       </c>
       <c r="H131" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I131" t="s" s="2">
         <v>74</v>
@@ -16591,7 +16609,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="132">
+    <row r="132" hidden="true">
       <c r="A132" t="s" s="2">
         <v>552</v>
       </c>
@@ -16701,7 +16719,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="133">
+    <row r="133" hidden="true">
       <c r="A133" t="s" s="2">
         <v>553</v>
       </c>
@@ -16811,7 +16829,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="134">
+    <row r="134" hidden="true">
       <c r="A134" t="s" s="2">
         <v>554</v>
       </c>
@@ -16832,7 +16850,7 @@
         <v>76</v>
       </c>
       <c r="H134" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I134" t="s" s="2">
         <v>74</v>
@@ -16919,7 +16937,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" hidden="true">
       <c r="A135" t="s" s="2">
         <v>558</v>
       </c>
@@ -17025,7 +17043,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="136">
+    <row r="136" hidden="true">
       <c r="A136" t="s" s="2">
         <v>559</v>
       </c>
@@ -17133,7 +17151,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="137">
+    <row r="137" hidden="true">
       <c r="A137" t="s" s="2">
         <v>560</v>
       </c>
@@ -17154,7 +17172,7 @@
         <v>75</v>
       </c>
       <c r="H137" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I137" t="s" s="2">
         <v>74</v>
@@ -17241,7 +17259,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="138">
+    <row r="138" hidden="true">
       <c r="A138" t="s" s="2">
         <v>561</v>
       </c>
@@ -17351,7 +17369,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" hidden="true">
       <c r="A139" t="s" s="2">
         <v>562</v>
       </c>
@@ -17461,7 +17479,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="140">
+    <row r="140" hidden="true">
       <c r="A140" t="s" s="2">
         <v>563</v>
       </c>
@@ -17482,7 +17500,7 @@
         <v>83</v>
       </c>
       <c r="H140" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I140" t="s" s="2">
         <v>74</v>
@@ -17569,7 +17587,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="141">
+    <row r="141" hidden="true">
       <c r="A141" t="s" s="2">
         <v>567</v>
       </c>
@@ -17675,7 +17693,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" hidden="true">
       <c r="A142" t="s" s="2">
         <v>568</v>
       </c>
@@ -17783,7 +17801,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" hidden="true">
       <c r="A143" t="s" s="2">
         <v>569</v>
       </c>
@@ -17804,7 +17822,7 @@
         <v>75</v>
       </c>
       <c r="H143" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I143" t="s" s="2">
         <v>74</v>
@@ -17891,7 +17909,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" hidden="true">
       <c r="A144" t="s" s="2">
         <v>570</v>
       </c>
@@ -18001,7 +18019,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" hidden="true">
       <c r="A145" t="s" s="2">
         <v>571</v>
       </c>
@@ -18111,7 +18129,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" hidden="true">
       <c r="A146" t="s" s="2">
         <v>572</v>
       </c>
@@ -18219,7 +18237,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" hidden="true">
       <c r="A147" t="s" s="2">
         <v>577</v>
       </c>
@@ -18327,7 +18345,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" hidden="true">
       <c r="A148" t="s" s="2">
         <v>582</v>
       </c>
@@ -18433,7 +18451,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" hidden="true">
       <c r="A149" t="s" s="2">
         <v>585</v>
       </c>
@@ -18452,7 +18470,7 @@
         <v>83</v>
       </c>
       <c r="H149" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I149" t="s" s="2">
         <v>74</v>
@@ -18541,7 +18559,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="150">
+    <row r="150" hidden="true">
       <c r="A150" t="s" s="2">
         <v>590</v>
       </c>
@@ -18647,7 +18665,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" hidden="true">
       <c r="A151" t="s" s="2">
         <v>591</v>
       </c>
@@ -18755,7 +18773,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" hidden="true">
       <c r="A152" t="s" s="2">
         <v>592</v>
       </c>
@@ -18776,7 +18794,7 @@
         <v>83</v>
       </c>
       <c r="H152" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I152" t="s" s="2">
         <v>74</v>
@@ -18863,7 +18881,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="153">
+    <row r="153" hidden="true">
       <c r="A153" t="s" s="2">
         <v>597</v>
       </c>
@@ -18884,7 +18902,7 @@
         <v>83</v>
       </c>
       <c r="H153" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I153" t="s" s="2">
         <v>74</v>
@@ -18971,7 +18989,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="154">
+    <row r="154" hidden="true">
       <c r="A154" t="s" s="2">
         <v>602</v>
       </c>
@@ -18992,7 +19010,7 @@
         <v>83</v>
       </c>
       <c r="H154" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I154" t="s" s="2">
         <v>74</v>
@@ -19079,7 +19097,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="155">
+    <row r="155" hidden="true">
       <c r="A155" t="s" s="2">
         <v>607</v>
       </c>
@@ -19189,7 +19207,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" hidden="true">
       <c r="A156" t="s" s="2">
         <v>608</v>
       </c>
@@ -19297,7 +19315,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" hidden="true">
       <c r="A157" t="s" s="2">
         <v>613</v>
       </c>
@@ -19403,7 +19421,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="158">
+    <row r="158" hidden="true">
       <c r="A158" t="s" s="2">
         <v>616</v>
       </c>
@@ -19511,7 +19529,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" hidden="true">
       <c r="A159" t="s" s="2">
         <v>621</v>
       </c>
@@ -19619,7 +19637,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="160">
+    <row r="160" hidden="true">
       <c r="A160" t="s" s="2">
         <v>624</v>
       </c>
@@ -19638,7 +19656,7 @@
         <v>76</v>
       </c>
       <c r="H160" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I160" t="s" s="2">
         <v>74</v>
@@ -19723,7 +19741,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" hidden="true">
       <c r="A161" t="s" s="2">
         <v>628</v>
       </c>
@@ -19829,7 +19847,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" hidden="true">
       <c r="A162" t="s" s="2">
         <v>629</v>
       </c>
@@ -19937,7 +19955,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" hidden="true">
       <c r="A163" t="s" s="2">
         <v>630</v>
       </c>
@@ -20047,7 +20065,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="164">
+    <row r="164" hidden="true">
       <c r="A164" t="s" s="2">
         <v>631</v>
       </c>
@@ -20155,7 +20173,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="165">
+    <row r="165" hidden="true">
       <c r="A165" t="s" s="2">
         <v>634</v>
       </c>
@@ -20263,7 +20281,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="166">
+    <row r="166" hidden="true">
       <c r="A166" t="s" s="2">
         <v>637</v>
       </c>
@@ -20284,7 +20302,7 @@
         <v>83</v>
       </c>
       <c r="H166" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I166" t="s" s="2">
         <v>74</v>
@@ -20371,7 +20389,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="167">
+    <row r="167" hidden="true">
       <c r="A167" t="s" s="2">
         <v>640</v>
       </c>
@@ -20477,7 +20495,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="168">
+    <row r="168" hidden="true">
       <c r="A168" t="s" s="2">
         <v>641</v>
       </c>
@@ -20585,7 +20603,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="169">
+    <row r="169" hidden="true">
       <c r="A169" t="s" s="2">
         <v>642</v>
       </c>
@@ -20695,7 +20713,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="170">
+    <row r="170" hidden="true">
       <c r="A170" t="s" s="2">
         <v>643</v>
       </c>
@@ -20803,7 +20821,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="171">
+    <row r="171" hidden="true">
       <c r="A171" t="s" s="2">
         <v>645</v>
       </c>
@@ -20911,7 +20929,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="172">
+    <row r="172" hidden="true">
       <c r="A172" t="s" s="2">
         <v>646</v>
       </c>
@@ -21017,7 +21035,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="173">
+    <row r="173" hidden="true">
       <c r="A173" t="s" s="2">
         <v>648</v>
       </c>
@@ -21125,7 +21143,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="174">
+    <row r="174" hidden="true">
       <c r="A174" t="s" s="2">
         <v>650</v>
       </c>
@@ -21233,7 +21251,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="175">
+    <row r="175" hidden="true">
       <c r="A175" t="s" s="2">
         <v>659</v>
       </c>
@@ -21343,7 +21361,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="176">
+    <row r="176" hidden="true">
       <c r="A176" t="s" s="2">
         <v>667</v>
       </c>
@@ -21451,7 +21469,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="177">
+    <row r="177" hidden="true">
       <c r="A177" t="s" s="2">
         <v>670</v>
       </c>
@@ -21560,6 +21578,24 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AL177">
+    <filterColumn colId="6">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="26">
+      <filters blank="true"/>
+    </filterColumn>
+  </autoFilter>
+  <conditionalFormatting sqref="A2:AI176">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$G2&lt;&gt;"Y"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$Q2&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sd ref ressources profils (#271)
* add ref profils
* suppr contrainte ref sur assigner 9e0cbbd3b3b6ace814c5b6f55cd8d57d6cf43732
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-ror-healthcareservice.xlsx
+++ b/main/ig/StructureDefinition-ror-healthcareservice.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-07T14:28:15+00:00</t>
+    <t>2024-02-07T16:04:22+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -800,7 +800,7 @@
     <t>HealthcareService.providedBy</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Organization)
+    <t xml:space="preserve">Reference(http://interopsante.org/fhir/StructureDefinition/FrOrganization|https://interop.esante.gouv.fr/ig/fhir/ror/StructureDefinition/ror-organization)
 </t>
   </si>
   <si>
@@ -917,7 +917,7 @@
     <t>HealthcareService.location</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Location)
+    <t xml:space="preserve">Reference(Location|https://interop.esante.gouv.fr/ig/fhir/ror/StructureDefinition/ror-location)
 </t>
   </si>
   <si>
@@ -2442,7 +2442,7 @@
     <col min="8" max="8" width="16.27734375" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.26171875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="112.875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="138.9140625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
add MS et def pour start et end (#311) bb60c867ae50b2adecc17cba164c73d838d87f2e
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-ror-healthcareservice.xlsx
+++ b/main/ig/StructureDefinition-ror-healthcareservice.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-11T15:45:47+00:00</t>
+    <t>2024-02-12T12:45:21+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1933,7 +1933,7 @@
 </t>
   </si>
   <si>
-    <t>Opening time of day (ignored if allDay = true)</t>
+    <t>heureDebut (Horaire) : Heure de début de la plage horaire</t>
   </si>
   <si>
     <t>The opening time of day. Note: If the AllDay flag is set, then this time is ignored.</t>
@@ -1945,7 +1945,7 @@
     <t>HealthcareService.availableTime.availableEndTime</t>
   </si>
   <si>
-    <t>Closing time of day (ignored if allDay = true)</t>
+    <t>heureFin (Horaire) : Heure de fin de la plage horaire</t>
   </si>
   <si>
     <t>The closing time of day. Note: If the AllDay flag is set, then this time is ignored.</t>
@@ -19440,7 +19440,7 @@
         <v>83</v>
       </c>
       <c r="H158" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I158" t="s" s="2">
         <v>74</v>
@@ -19548,7 +19548,7 @@
         <v>83</v>
       </c>
       <c r="H159" t="s" s="2">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="I159" t="s" s="2">
         <v>74</v>

</xml_diff>

<commit_message>
add PUT pour questionnaire (#400) 726cb9e6b7320f31ea823baa975ada465b141da7
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-ror-healthcareservice.xlsx
+++ b/main/ig/StructureDefinition-ror-healthcareservice.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-01-28T15:58:19+00:00</t>
+    <t>2025-03-03T10:17:50+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -12697,10 +12697,10 @@
         <v>85</v>
       </c>
       <c r="G92" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="H92" t="s" s="2">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="I92" t="s" s="2">
         <v>75</v>
@@ -12709,13 +12709,13 @@
         <v>75</v>
       </c>
       <c r="K92" t="s" s="2">
-        <v>110</v>
+        <v>446</v>
       </c>
       <c r="L92" t="s" s="2">
-        <v>198</v>
+        <v>447</v>
       </c>
       <c r="M92" t="s" s="2">
-        <v>199</v>
+        <v>448</v>
       </c>
       <c r="N92" s="2"/>
       <c r="O92" s="2"/>
@@ -13799,10 +13799,10 @@
         <v>85</v>
       </c>
       <c r="G102" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="H102" t="s" s="2">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="I102" t="s" s="2">
         <v>75</v>
@@ -13811,13 +13811,13 @@
         <v>75</v>
       </c>
       <c r="K102" t="s" s="2">
-        <v>110</v>
+        <v>446</v>
       </c>
       <c r="L102" t="s" s="2">
-        <v>198</v>
+        <v>447</v>
       </c>
       <c r="M102" t="s" s="2">
-        <v>199</v>
+        <v>448</v>
       </c>
       <c r="N102" s="2"/>
       <c r="O102" s="2"/>

</xml_diff>

<commit_message>
Add comment to Location and LocationSupportedCapacity (#440)
* add comment to location and location-supported-capactity

* rename RORLocationComment to RORComment f53e6752c13fdb3467088d60501c8009bfffa804
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-ror-healthcareservice.xlsx
+++ b/main/ig/StructureDefinition-ror-healthcareservice.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-30T09:38:37+00:00</t>
+    <t>2025-10-16T15:18:57+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -947,7 +947,7 @@
     <t>operationalActivityFamily</t>
   </si>
   <si>
-    <t>familleActiviteOperationnelle (ActiviteOperationnelle) : regroupement cohérent d’activités délivrées dans le cadre d'une prestation, répondant à un besoin de la personne</t>
+    <t>familleActiviteOperationnelle (ActiviteOperationnelle) : dans le secteur médico-social, la famille d’activité correspond au niveau 4 des prestations de la nomenclature SERAFIN</t>
   </si>
   <si>
     <t>https://mos.esante.gouv.fr/NOS/JDV_J51-FamilleActiviteOperationnelle-ROR/FHIR/JDV-J51-FamilleActiviteOperationnelle-ROR</t>
@@ -5703,7 +5703,7 @@
       </c>
       <c r="E29" s="2"/>
       <c r="F29" t="s" s="2">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="G29" t="s" s="2">
         <v>85</v>
@@ -20239,7 +20239,7 @@
         <v>76</v>
       </c>
       <c r="G160" t="s" s="2">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="H160" t="s" s="2">
         <v>86</v>

</xml_diff>